<commit_message>
Struggling with convolution matrix
</commit_message>
<xml_diff>
--- a/matrices.xlsx
+++ b/matrices.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arc/Research/PhD/Projects/supy-res-imaging/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52977303-BF70-9E45-A3CF-01C43784D61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65123339-4F34-BF49-A6B3-E250D1B2595B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="44800" windowHeight="24700" xr2:uid="{BFB4648C-04C2-8441-A657-02EBE8D5E21E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="24700" activeTab="1" xr2:uid="{BFB4648C-04C2-8441-A657-02EBE8D5E21E}"/>
   </bookViews>
   <sheets>
     <sheet name="Decimation Matrix" sheetId="1" r:id="rId1"/>
+    <sheet name="Sharpening Matrix" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="7">
   <si>
     <t>High-res image dim</t>
   </si>
@@ -47,6 +48,15 @@
   </si>
   <si>
     <t>D matrix height</t>
+  </si>
+  <si>
+    <t>Matrix Dim</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
 </sst>
 </file>
@@ -321,7 +331,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -644,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FA45D9A-981D-214F-9028-128C4FDDE46C}">
   <dimension ref="A1:BV35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13:T13"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4578,7 +4598,7 @@
         <color rgb="FF92D050"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4595,4 +4615,593 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4E2BDF2-F335-BB46-BAC5-D1F6DABDF64C}">
+  <dimension ref="A1:T27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="211" zoomScaleNormal="211" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="20" width="4.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="10">
+        <v>0</v>
+      </c>
+      <c r="F2" s="10">
+        <f>E2+1</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="10">
+        <f t="shared" ref="G2:T2" si="0">F2+1</f>
+        <v>2</v>
+      </c>
+      <c r="H2" s="10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I2" s="10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J2" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K2" s="10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L2" s="10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="M2" s="10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="N2" s="10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="O2" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="P2" s="10">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="Q2" s="10">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="R2" s="10">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="S2" s="10">
+        <f>R2+1</f>
+        <v>14</v>
+      </c>
+      <c r="T2" s="10">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D3" s="10">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="4"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D4" s="10">
+        <f>D3+1</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="6"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D5" s="10">
+        <f t="shared" ref="D5:D18" si="1">D4+1</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="6"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D6" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="6"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D7" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="6"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D8" s="10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="6"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D9" s="10">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="6"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D10" s="10">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="6"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D11" s="10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="6"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D12" s="10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="6"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D13" s="10">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="6"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D14" s="10">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="6"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D15" s="10">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="6"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D16" s="10">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="6"/>
+    </row>
+    <row r="17" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D17" s="10">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="6"/>
+    </row>
+    <row r="18" spans="4:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="10">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="P18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="T18" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="4:20" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D20" s="10"/>
+      <c r="E20">
+        <v>-2</v>
+      </c>
+      <c r="F20">
+        <f>E20+1</f>
+        <v>-1</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ref="G20:J20" si="2">F20+1</f>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>-2</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="4:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f>D21+1</f>
+        <v>-1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="4:20" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <f t="shared" ref="D23:D26" si="3">D22+1</f>
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="4:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="9"/>
+    </row>
+    <row r="27" spans="4:20" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>